<commit_message>
registerUser function added to BusinessAction class
</commit_message>
<xml_diff>
--- a/java/Hybrid/util/TestSuit.xlsx
+++ b/java/Hybrid/util/TestSuit.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="57">
   <si>
     <t xml:space="preserve">Test Scenario</t>
   </si>
@@ -43,7 +43,7 @@
     <t xml:space="preserve">“1434”</t>
   </si>
   <si>
-    <t xml:space="preserve">YES</t>
+    <t xml:space="preserve">NO</t>
   </si>
   <si>
     <t xml:space="preserve">login</t>
@@ -147,9 +147,6 @@
     <t xml:space="preserve">“ ”</t>
   </si>
   <si>
-    <t xml:space="preserve">NO</t>
-  </si>
-  <si>
     <t xml:space="preserve">checking checkout</t>
   </si>
   <si>
@@ -169,6 +166,33 @@
   </si>
   <si>
     <t xml:space="preserve">checking checkout page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">checking cart check</t>
+  </si>
+  <si>
+    <t xml:space="preserve">checking BUY NOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">productDetailPageBuyNow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">checking search</t>
+  </si>
+  <si>
+    <t xml:space="preserve">checking search with sort</t>
+  </si>
+  <si>
+    <t xml:space="preserve">searchSort</t>
+  </si>
+  <si>
+    <t xml:space="preserve">checking Register</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">registerUser</t>
   </si>
 </sst>
 </file>
@@ -317,29 +341,30 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P19"/>
+  <dimension ref="A1:P24"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E21" activeCellId="0" sqref="E21"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.5255102040816"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.5969387755102"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.3112244897959"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.9489795918367"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.6530612244898"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -657,7 +682,7 @@
         <v>40</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>41</v>
+        <v>7</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>35</v>
@@ -665,13 +690,13 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B15" s="0" t="s">
         <v>25</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>41</v>
+        <v>7</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>8</v>
@@ -703,13 +728,13 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B16" s="0" t="s">
         <v>25</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>41</v>
+        <v>7</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>8</v>
@@ -735,13 +760,13 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="C17" s="2" t="s">
-        <v>41</v>
+        <v>7</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>11</v>
@@ -761,36 +786,122 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B18" s="0" t="s">
         <v>25</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>41</v>
+        <v>7</v>
       </c>
       <c r="D18" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B19" s="0" t="s">
         <v>25</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>41</v>
+        <v>7</v>
       </c>
       <c r="D19" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E19" s="0" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F21" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G21" s="5"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>